<commit_message>
H3 en principi arreglada
PROS: JA VA AMB EL TESTEADOR I LO DE TREURE ELAS QUE SOBREN

CONTRAS: NO PASSA NI EN 1 EXEMPLAR LA QUALITAT MINIMA
</commit_message>
<xml_diff>
--- a/PROVA.xlsx
+++ b/PROVA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maria\Desktop\MASTER\_Q3cuc\MÈTODES QUANTITATIUS D'ORGANITZACIÓ INDUSTRIAL II\Treball d'avaluació\Entrega parcial del programa informàtic\program_parcial\mqoi2-algo-parcial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DEC682E-A96F-4307-B3C7-AA4F7FEA5098}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089E376E-E744-4C0F-A3D8-3BED8506BB18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{DD10B349-A6DC-41D0-A261-0581506FDB24}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="235">
   <si>
     <t>0*1*0*1</t>
   </si>
@@ -441,6 +440,297 @@
   </si>
   <si>
     <t>NOM</t>
+  </si>
+  <si>
+    <t>376000.0</t>
+  </si>
+  <si>
+    <t>229000.0</t>
+  </si>
+  <si>
+    <t>151500.0</t>
+  </si>
+  <si>
+    <t>414500.0</t>
+  </si>
+  <si>
+    <t>466500.0</t>
+  </si>
+  <si>
+    <t>443500.0</t>
+  </si>
+  <si>
+    <t>287000.0</t>
+  </si>
+  <si>
+    <t>145000.0</t>
+  </si>
+  <si>
+    <t>419500.0</t>
+  </si>
+  <si>
+    <t>341500.0</t>
+  </si>
+  <si>
+    <t>244000.0</t>
+  </si>
+  <si>
+    <t>316500.0</t>
+  </si>
+  <si>
+    <t>294000.0</t>
+  </si>
+  <si>
+    <t>206500.0</t>
+  </si>
+  <si>
+    <t>271000.0</t>
+  </si>
+  <si>
+    <t>245000.0</t>
+  </si>
+  <si>
+    <t>298000.0</t>
+  </si>
+  <si>
+    <t>142000.0</t>
+  </si>
+  <si>
+    <t>210000.0</t>
+  </si>
+  <si>
+    <t>385500.0</t>
+  </si>
+  <si>
+    <t>463000.0</t>
+  </si>
+  <si>
+    <t>219000.0</t>
+  </si>
+  <si>
+    <t>196500.0</t>
+  </si>
+  <si>
+    <t>364500.0</t>
+  </si>
+  <si>
+    <t>194000.0</t>
+  </si>
+  <si>
+    <t>175000.0</t>
+  </si>
+  <si>
+    <t>237000.0</t>
+  </si>
+  <si>
+    <t>317500.0</t>
+  </si>
+  <si>
+    <t>146500.0</t>
+  </si>
+  <si>
+    <t>270000.0</t>
+  </si>
+  <si>
+    <t>345500.0</t>
+  </si>
+  <si>
+    <t>174500.0</t>
+  </si>
+  <si>
+    <t>321000.0</t>
+  </si>
+  <si>
+    <t>191000.0</t>
+  </si>
+  <si>
+    <t>383500.0</t>
+  </si>
+  <si>
+    <t>485000.0</t>
+  </si>
+  <si>
+    <t>515000.0</t>
+  </si>
+  <si>
+    <t>343000.0</t>
+  </si>
+  <si>
+    <t>216000.0</t>
+  </si>
+  <si>
+    <t>451500.0</t>
+  </si>
+  <si>
+    <t>296000.0</t>
+  </si>
+  <si>
+    <t>306500.0</t>
+  </si>
+  <si>
+    <t>147500.0</t>
+  </si>
+  <si>
+    <t>277500.0</t>
+  </si>
+  <si>
+    <t>254000.0</t>
+  </si>
+  <si>
+    <t>233000.0</t>
+  </si>
+  <si>
+    <t>422500.0</t>
+  </si>
+  <si>
+    <t>390500.0</t>
+  </si>
+  <si>
+    <t>289500.0</t>
+  </si>
+  <si>
+    <t>259000.0</t>
+  </si>
+  <si>
+    <t>432500.0</t>
+  </si>
+  <si>
+    <t>139000.0</t>
+  </si>
+  <si>
+    <t>123500.0</t>
+  </si>
+  <si>
+    <t>285000.0</t>
+  </si>
+  <si>
+    <t>421500.0</t>
+  </si>
+  <si>
+    <t>308500.0</t>
+  </si>
+  <si>
+    <t>150000.0</t>
+  </si>
+  <si>
+    <t>319000.0</t>
+  </si>
+  <si>
+    <t>341000.0</t>
+  </si>
+  <si>
+    <t>415500.0</t>
+  </si>
+  <si>
+    <t>230000.0</t>
+  </si>
+  <si>
+    <t>433500.0</t>
+  </si>
+  <si>
+    <t>491500.0</t>
+  </si>
+  <si>
+    <t>259500.0</t>
+  </si>
+  <si>
+    <t>381000.0</t>
+  </si>
+  <si>
+    <t>481500.0</t>
+  </si>
+  <si>
+    <t>235500.0</t>
+  </si>
+  <si>
+    <t>359000.0</t>
+  </si>
+  <si>
+    <t>286000.0</t>
+  </si>
+  <si>
+    <t>468500.0</t>
+  </si>
+  <si>
+    <t>372000.0</t>
+  </si>
+  <si>
+    <t>234500.0</t>
+  </si>
+  <si>
+    <t>292500.0</t>
+  </si>
+  <si>
+    <t>358000.0</t>
+  </si>
+  <si>
+    <t>342000.0</t>
+  </si>
+  <si>
+    <t>327000.0</t>
+  </si>
+  <si>
+    <t>511000.0</t>
+  </si>
+  <si>
+    <t>243000.0</t>
+  </si>
+  <si>
+    <t>170000.0</t>
+  </si>
+  <si>
+    <t>172000.0</t>
+  </si>
+  <si>
+    <t>478500.0</t>
+  </si>
+  <si>
+    <t>458000.0</t>
+  </si>
+  <si>
+    <t>386500.0</t>
+  </si>
+  <si>
+    <t>240000.0</t>
+  </si>
+  <si>
+    <t>526000.0</t>
+  </si>
+  <si>
+    <t>360500.0</t>
+  </si>
+  <si>
+    <t>149500.0</t>
+  </si>
+  <si>
+    <t>272000.0</t>
+  </si>
+  <si>
+    <t>345000.0</t>
+  </si>
+  <si>
+    <t>344000.0</t>
+  </si>
+  <si>
+    <t>465000.0</t>
+  </si>
+  <si>
+    <t>378500.0</t>
+  </si>
+  <si>
+    <t>362000.0</t>
+  </si>
+  <si>
+    <t>282500.0</t>
+  </si>
+  <si>
+    <t>340000.0</t>
+  </si>
+  <si>
+    <t>nostre2</t>
+  </si>
+  <si>
+    <t>dins2</t>
   </si>
 </sst>
 </file>
@@ -491,7 +781,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -503,13 +793,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFC4A4A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3099,10 +3382,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF627B8D-0597-490A-89E4-9C0199E84F53}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D2" sqref="D2:D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,9 +3393,10 @@
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>137</v>
       </c>
@@ -3123,10 +3407,16 @@
         <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -3134,14 +3424,21 @@
         <v>356500</v>
       </c>
       <c r="C2">
-        <v>339900</v>
-      </c>
-      <c r="D2" t="b">
+        <v>377500</v>
+      </c>
+      <c r="D2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" t="b">
         <f>C2&lt;B2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <f>D2&lt;C2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3149,14 +3446,21 @@
         <v>215500</v>
       </c>
       <c r="C3">
-        <v>191900</v>
-      </c>
-      <c r="D3" t="b">
-        <f t="shared" ref="D3:D66" si="0">C3&lt;B3</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>229000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="b">
+        <f t="shared" ref="E3:E66" si="0">C3&lt;B3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <f t="shared" ref="F3:F66" si="1">D3&lt;C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3164,14 +3468,21 @@
         <v>141000</v>
       </c>
       <c r="C4">
-        <v>108900</v>
-      </c>
-      <c r="D4" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>151500</v>
+      </c>
+      <c r="D4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E4" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -3179,14 +3490,21 @@
         <v>395500</v>
       </c>
       <c r="C5">
-        <v>373800</v>
-      </c>
-      <c r="D5" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>414500</v>
+      </c>
+      <c r="D5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -3194,14 +3512,21 @@
         <v>443500</v>
       </c>
       <c r="C6">
-        <v>426300</v>
-      </c>
-      <c r="D6" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>466500</v>
+      </c>
+      <c r="D6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -3209,14 +3534,21 @@
         <v>418500</v>
       </c>
       <c r="C7">
-        <v>384600</v>
-      </c>
-      <c r="D7" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>443500</v>
+      </c>
+      <c r="D7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -3224,14 +3556,21 @@
         <v>271000</v>
       </c>
       <c r="C8">
-        <v>239800</v>
-      </c>
-      <c r="D8" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>287000</v>
+      </c>
+      <c r="D8" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -3239,14 +3578,21 @@
         <v>137500</v>
       </c>
       <c r="C9">
-        <v>141400</v>
-      </c>
-      <c r="D9" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -3254,14 +3600,21 @@
         <v>396500</v>
       </c>
       <c r="C10">
-        <v>358600</v>
-      </c>
-      <c r="D10" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>421000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -3269,14 +3622,21 @@
         <v>322000</v>
       </c>
       <c r="C11">
-        <v>280600</v>
-      </c>
-      <c r="D11" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>341500</v>
+      </c>
+      <c r="D11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -3284,14 +3644,21 @@
         <v>232500</v>
       </c>
       <c r="C12">
-        <v>221600</v>
-      </c>
-      <c r="D12" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245500</v>
+      </c>
+      <c r="D12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -3299,14 +3666,21 @@
         <v>297000</v>
       </c>
       <c r="C13">
-        <v>254100</v>
-      </c>
-      <c r="D13" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>316500</v>
+      </c>
+      <c r="D13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F13" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -3314,14 +3688,21 @@
         <v>275500</v>
       </c>
       <c r="C14">
-        <v>223000</v>
-      </c>
-      <c r="D14" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>294000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -3329,14 +3710,21 @@
         <v>192500</v>
       </c>
       <c r="C15">
-        <v>172500</v>
-      </c>
-      <c r="D15" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>206500</v>
+      </c>
+      <c r="D15" t="s">
+        <v>151</v>
+      </c>
+      <c r="E15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -3344,14 +3732,21 @@
         <v>255500</v>
       </c>
       <c r="C16">
-        <v>260800</v>
-      </c>
-      <c r="D16" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>271000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F16" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -3359,14 +3754,21 @@
         <v>231500</v>
       </c>
       <c r="C17">
-        <v>221100</v>
-      </c>
-      <c r="D17" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>245000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -3374,14 +3776,21 @@
         <v>282000</v>
       </c>
       <c r="C18">
-        <v>245700</v>
-      </c>
-      <c r="D18" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>298000</v>
+      </c>
+      <c r="D18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E18" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -3389,14 +3798,21 @@
         <v>133000</v>
       </c>
       <c r="C19">
-        <v>108000</v>
-      </c>
-      <c r="D19" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>142000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -3404,14 +3820,21 @@
         <v>197000</v>
       </c>
       <c r="C20">
-        <v>169400</v>
-      </c>
-      <c r="D20" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>210000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -3419,14 +3842,21 @@
         <v>363000</v>
       </c>
       <c r="C21">
-        <v>324600</v>
-      </c>
-      <c r="D21" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>385500</v>
+      </c>
+      <c r="D21" t="s">
+        <v>157</v>
+      </c>
+      <c r="E21" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -3434,14 +3864,21 @@
         <v>435500</v>
       </c>
       <c r="C22">
-        <v>379800</v>
-      </c>
-      <c r="D22" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>463000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>158</v>
+      </c>
+      <c r="E22" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -3449,14 +3886,21 @@
         <v>207000</v>
       </c>
       <c r="C23">
-        <v>195100</v>
-      </c>
-      <c r="D23" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>219000</v>
+      </c>
+      <c r="D23" t="s">
+        <v>159</v>
+      </c>
+      <c r="E23" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -3464,14 +3908,21 @@
         <v>181500</v>
       </c>
       <c r="C24">
-        <v>132600</v>
-      </c>
-      <c r="D24" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>197000</v>
+      </c>
+      <c r="D24" t="s">
+        <v>160</v>
+      </c>
+      <c r="E24" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -3479,14 +3930,21 @@
         <v>344500</v>
       </c>
       <c r="C25">
-        <v>342600</v>
-      </c>
-      <c r="D25" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>364500</v>
+      </c>
+      <c r="D25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -3494,14 +3952,21 @@
         <v>183000</v>
       </c>
       <c r="C26">
-        <v>131100</v>
-      </c>
-      <c r="D26" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>194000</v>
+      </c>
+      <c r="D26" t="s">
+        <v>162</v>
+      </c>
+      <c r="E26" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -3509,14 +3974,21 @@
         <v>163000</v>
       </c>
       <c r="C27">
-        <v>141000</v>
-      </c>
-      <c r="D27" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>175000</v>
+      </c>
+      <c r="D27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F27" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -3524,14 +3996,21 @@
         <v>224000</v>
       </c>
       <c r="C28">
-        <v>197900</v>
-      </c>
-      <c r="D28" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>237000</v>
+      </c>
+      <c r="D28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E28" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F28" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -3539,14 +4018,21 @@
         <v>297500</v>
       </c>
       <c r="C29">
-        <v>256600</v>
-      </c>
-      <c r="D29" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>317500</v>
+      </c>
+      <c r="D29" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>65</v>
       </c>
@@ -3554,14 +4040,21 @@
         <v>192500</v>
       </c>
       <c r="C30">
-        <v>189200</v>
-      </c>
-      <c r="D30" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>208000</v>
+      </c>
+      <c r="D30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E30" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -3569,14 +4062,21 @@
         <v>136500</v>
       </c>
       <c r="C31">
-        <v>97300</v>
-      </c>
-      <c r="D31" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>146500</v>
+      </c>
+      <c r="D31" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -3584,14 +4084,21 @@
         <v>256000</v>
       </c>
       <c r="C32">
-        <v>224300</v>
-      </c>
-      <c r="D32" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>270000</v>
+      </c>
+      <c r="D32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E32" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>68</v>
       </c>
@@ -3599,14 +4106,21 @@
         <v>325000</v>
       </c>
       <c r="C33">
-        <v>288700</v>
-      </c>
-      <c r="D33" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>346000</v>
+      </c>
+      <c r="D33" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -3614,14 +4128,21 @@
         <v>163000</v>
       </c>
       <c r="C34">
-        <v>132400</v>
-      </c>
-      <c r="D34" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>174500</v>
+      </c>
+      <c r="D34" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>70</v>
       </c>
@@ -3629,14 +4150,21 @@
         <v>304500</v>
       </c>
       <c r="C35">
-        <v>285400</v>
-      </c>
-      <c r="D35" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>321000</v>
+      </c>
+      <c r="D35" t="s">
+        <v>170</v>
+      </c>
+      <c r="E35" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -3644,14 +4172,21 @@
         <v>180500</v>
       </c>
       <c r="C36">
-        <v>150400</v>
-      </c>
-      <c r="D36" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>191000</v>
+      </c>
+      <c r="D36" t="s">
+        <v>171</v>
+      </c>
+      <c r="E36" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -3659,14 +4194,21 @@
         <v>362000</v>
       </c>
       <c r="C37">
-        <v>346400</v>
-      </c>
-      <c r="D37" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>383500</v>
+      </c>
+      <c r="D37" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -3674,14 +4216,21 @@
         <v>458500</v>
       </c>
       <c r="C38">
-        <v>437700</v>
-      </c>
-      <c r="D38" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>485000</v>
+      </c>
+      <c r="D38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -3689,14 +4238,21 @@
         <v>484500</v>
       </c>
       <c r="C39">
-        <v>407400</v>
-      </c>
-      <c r="D39" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>515000</v>
+      </c>
+      <c r="D39" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -3704,14 +4260,21 @@
         <v>321500</v>
       </c>
       <c r="C40">
-        <v>293800</v>
-      </c>
-      <c r="D40" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>343000</v>
+      </c>
+      <c r="D40" t="s">
+        <v>175</v>
+      </c>
+      <c r="E40" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F40" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -3719,14 +4282,21 @@
         <v>199500</v>
       </c>
       <c r="C41">
-        <v>166300</v>
-      </c>
-      <c r="D41" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>217000</v>
+      </c>
+      <c r="D41" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -3734,14 +4304,21 @@
         <v>427000</v>
       </c>
       <c r="C42">
-        <v>371800</v>
-      </c>
-      <c r="D42" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>451500</v>
+      </c>
+      <c r="D42" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F42" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -3749,14 +4326,21 @@
         <v>276500</v>
       </c>
       <c r="C43">
-        <v>260500</v>
-      </c>
-      <c r="D43" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>296000</v>
+      </c>
+      <c r="D43" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F43" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -3764,14 +4348,21 @@
         <v>287500</v>
       </c>
       <c r="C44">
-        <v>283100</v>
-      </c>
-      <c r="D44" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>306500</v>
+      </c>
+      <c r="D44" t="s">
+        <v>179</v>
+      </c>
+      <c r="E44" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -3779,14 +4370,21 @@
         <v>139000</v>
       </c>
       <c r="C45">
-        <v>128700</v>
-      </c>
-      <c r="D45" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>147500</v>
+      </c>
+      <c r="D45" t="s">
+        <v>180</v>
+      </c>
+      <c r="E45" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F45" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -3794,14 +4392,21 @@
         <v>262500</v>
       </c>
       <c r="C46">
-        <v>218100</v>
-      </c>
-      <c r="D46" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>277500</v>
+      </c>
+      <c r="D46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E46" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F46" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -3809,14 +4414,21 @@
         <v>237500</v>
       </c>
       <c r="C47">
-        <v>211900</v>
-      </c>
-      <c r="D47" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>254000</v>
+      </c>
+      <c r="D47" t="s">
+        <v>182</v>
+      </c>
+      <c r="E47" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F47" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -3824,14 +4436,21 @@
         <v>218500</v>
       </c>
       <c r="C48">
-        <v>192400</v>
-      </c>
-      <c r="D48" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233000</v>
+      </c>
+      <c r="D48" t="s">
+        <v>183</v>
+      </c>
+      <c r="E48" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F48" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -3839,14 +4458,21 @@
         <v>397500</v>
       </c>
       <c r="C49">
-        <v>371700</v>
-      </c>
-      <c r="D49" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>422500</v>
+      </c>
+      <c r="D49" t="s">
+        <v>184</v>
+      </c>
+      <c r="E49" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F49" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -3854,14 +4480,21 @@
         <v>367000</v>
       </c>
       <c r="C50">
-        <v>291100</v>
-      </c>
-      <c r="D50" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>392500</v>
+      </c>
+      <c r="D50" t="s">
+        <v>185</v>
+      </c>
+      <c r="E50" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -3869,14 +4502,21 @@
         <v>274000</v>
       </c>
       <c r="C51">
-        <v>243300</v>
-      </c>
-      <c r="D51" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>291000</v>
+      </c>
+      <c r="D51" t="s">
+        <v>186</v>
+      </c>
+      <c r="E51" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F51" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -3884,14 +4524,21 @@
         <v>243000</v>
       </c>
       <c r="C52">
-        <v>203200</v>
-      </c>
-      <c r="D52" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>259000</v>
+      </c>
+      <c r="D52" t="s">
+        <v>187</v>
+      </c>
+      <c r="E52" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F52" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -3899,14 +4546,21 @@
         <v>409000</v>
       </c>
       <c r="C53">
-        <v>357900</v>
-      </c>
-      <c r="D53" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>434000</v>
+      </c>
+      <c r="D53" t="s">
+        <v>188</v>
+      </c>
+      <c r="E53" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F53" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>89</v>
       </c>
@@ -3914,14 +4568,21 @@
         <v>130500</v>
       </c>
       <c r="C54">
-        <v>115100</v>
-      </c>
-      <c r="D54" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139000</v>
+      </c>
+      <c r="D54" t="s">
+        <v>189</v>
+      </c>
+      <c r="E54" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F54" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -3929,14 +4590,21 @@
         <v>272000</v>
       </c>
       <c r="C55">
-        <v>242300</v>
-      </c>
-      <c r="D55" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>289500</v>
+      </c>
+      <c r="D55" t="s">
+        <v>186</v>
+      </c>
+      <c r="E55" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>91</v>
       </c>
@@ -3944,14 +4612,21 @@
         <v>114500</v>
       </c>
       <c r="C56">
-        <v>95100</v>
-      </c>
-      <c r="D56" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124000</v>
+      </c>
+      <c r="D56" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F56" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -3959,14 +4634,21 @@
         <v>268000</v>
       </c>
       <c r="C57">
-        <v>228200</v>
-      </c>
-      <c r="D57" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>287500</v>
+      </c>
+      <c r="D57" t="s">
+        <v>191</v>
+      </c>
+      <c r="E57" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -3974,14 +4656,21 @@
         <v>397500</v>
       </c>
       <c r="C58">
-        <v>355500</v>
-      </c>
-      <c r="D58" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>421500</v>
+      </c>
+      <c r="D58" t="s">
+        <v>192</v>
+      </c>
+      <c r="E58" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -3989,14 +4678,21 @@
         <v>291000</v>
       </c>
       <c r="C59">
-        <v>271400</v>
-      </c>
-      <c r="D59" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>308500</v>
+      </c>
+      <c r="D59" t="s">
+        <v>193</v>
+      </c>
+      <c r="E59" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F59" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -4004,14 +4700,21 @@
         <v>140500</v>
       </c>
       <c r="C60">
-        <v>107400</v>
-      </c>
-      <c r="D60" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>151500</v>
+      </c>
+      <c r="D60" t="s">
+        <v>194</v>
+      </c>
+      <c r="E60" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F60" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -4019,14 +4722,21 @@
         <v>325000</v>
       </c>
       <c r="C61">
-        <v>299800</v>
-      </c>
-      <c r="D61" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>345500</v>
+      </c>
+      <c r="D61" t="s">
+        <v>168</v>
+      </c>
+      <c r="E61" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F61" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -4034,14 +4744,21 @@
         <v>299000</v>
       </c>
       <c r="C62">
-        <v>293600</v>
-      </c>
-      <c r="D62" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>319000</v>
+      </c>
+      <c r="D62" t="s">
+        <v>195</v>
+      </c>
+      <c r="E62" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F62" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -4049,14 +4766,21 @@
         <v>321000</v>
       </c>
       <c r="C63">
-        <v>288700</v>
-      </c>
-      <c r="D63" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>341000</v>
+      </c>
+      <c r="D63" t="s">
+        <v>196</v>
+      </c>
+      <c r="E63" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F63" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>99</v>
       </c>
@@ -4064,14 +4788,21 @@
         <v>391000</v>
       </c>
       <c r="C64">
-        <v>323700</v>
-      </c>
-      <c r="D64" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>415500</v>
+      </c>
+      <c r="D64" t="s">
+        <v>197</v>
+      </c>
+      <c r="E64" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F64" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>100</v>
       </c>
@@ -4079,14 +4810,21 @@
         <v>214000</v>
       </c>
       <c r="C65">
-        <v>194500</v>
-      </c>
-      <c r="D65" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>230000</v>
+      </c>
+      <c r="D65" t="s">
+        <v>198</v>
+      </c>
+      <c r="E65" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F65" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -4094,14 +4832,21 @@
         <v>406500</v>
       </c>
       <c r="C66">
-        <v>357400</v>
-      </c>
-      <c r="D66" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>433500</v>
+      </c>
+      <c r="D66" t="s">
+        <v>199</v>
+      </c>
+      <c r="E66" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F66" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -4109,14 +4854,21 @@
         <v>463500</v>
       </c>
       <c r="C67">
-        <v>406300</v>
-      </c>
-      <c r="D67" t="b">
-        <f t="shared" ref="D67:D101" si="1">C67&lt;B67</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>494000</v>
+      </c>
+      <c r="D67" t="s">
+        <v>200</v>
+      </c>
+      <c r="E67" t="b">
+        <f t="shared" ref="E67:E101" si="2">C67&lt;B67</f>
+        <v>0</v>
+      </c>
+      <c r="F67" t="b">
+        <f t="shared" ref="F67:F101" si="3">D67&lt;C67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>103</v>
       </c>
@@ -4124,14 +4876,21 @@
         <v>245000</v>
       </c>
       <c r="C68">
-        <v>229000</v>
-      </c>
-      <c r="D68" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>259500</v>
+      </c>
+      <c r="D68" t="s">
+        <v>201</v>
+      </c>
+      <c r="E68" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F68" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>104</v>
       </c>
@@ -4139,14 +4898,21 @@
         <v>360500</v>
       </c>
       <c r="C69">
-        <v>354000</v>
-      </c>
-      <c r="D69" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>381000</v>
+      </c>
+      <c r="D69" t="s">
+        <v>202</v>
+      </c>
+      <c r="E69" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F69" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>105</v>
       </c>
@@ -4154,14 +4920,21 @@
         <v>453000</v>
       </c>
       <c r="C70">
-        <v>422600</v>
-      </c>
-      <c r="D70" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>481500</v>
+      </c>
+      <c r="D70" t="s">
+        <v>203</v>
+      </c>
+      <c r="E70" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F70" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>106</v>
       </c>
@@ -4169,14 +4942,21 @@
         <v>220500</v>
       </c>
       <c r="C71">
-        <v>201500</v>
-      </c>
-      <c r="D71" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>235500</v>
+      </c>
+      <c r="D71" t="s">
+        <v>204</v>
+      </c>
+      <c r="E71" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F71" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>107</v>
       </c>
@@ -4184,14 +4964,21 @@
         <v>337500</v>
       </c>
       <c r="C72">
-        <v>305200</v>
-      </c>
-      <c r="D72" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>359000</v>
+      </c>
+      <c r="D72" t="s">
+        <v>205</v>
+      </c>
+      <c r="E72" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F72" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>108</v>
       </c>
@@ -4199,14 +4986,21 @@
         <v>267000</v>
       </c>
       <c r="C73">
-        <v>252000</v>
-      </c>
-      <c r="D73" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>286000</v>
+      </c>
+      <c r="D73" t="s">
+        <v>206</v>
+      </c>
+      <c r="E73" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F73" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>109</v>
       </c>
@@ -4214,14 +5008,21 @@
         <v>441000</v>
       </c>
       <c r="C74">
-        <v>386800</v>
-      </c>
-      <c r="D74" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>469500</v>
+      </c>
+      <c r="D74" t="s">
+        <v>207</v>
+      </c>
+      <c r="E74" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F74" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>110</v>
       </c>
@@ -4229,14 +5030,21 @@
         <v>353000</v>
       </c>
       <c r="C75">
-        <v>317700</v>
-      </c>
-      <c r="D75" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>372000</v>
+      </c>
+      <c r="D75" t="s">
+        <v>208</v>
+      </c>
+      <c r="E75" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F75" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>111</v>
       </c>
@@ -4244,14 +5052,21 @@
         <v>218000</v>
       </c>
       <c r="C76">
-        <v>184800</v>
-      </c>
-      <c r="D76" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>235500</v>
+      </c>
+      <c r="D76" t="s">
+        <v>209</v>
+      </c>
+      <c r="E76" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F76" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>112</v>
       </c>
@@ -4259,14 +5074,21 @@
         <v>274500</v>
       </c>
       <c r="C77">
-        <v>260000</v>
-      </c>
-      <c r="D77" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>292500</v>
+      </c>
+      <c r="D77" t="s">
+        <v>210</v>
+      </c>
+      <c r="E77" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F77" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>113</v>
       </c>
@@ -4274,14 +5096,21 @@
         <v>339000</v>
       </c>
       <c r="C78">
-        <v>320900</v>
-      </c>
-      <c r="D78" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>358000</v>
+      </c>
+      <c r="D78" t="s">
+        <v>211</v>
+      </c>
+      <c r="E78" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F78" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>114</v>
       </c>
@@ -4289,14 +5118,21 @@
         <v>319000</v>
       </c>
       <c r="C79">
-        <v>286200</v>
-      </c>
-      <c r="D79" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>342000</v>
+      </c>
+      <c r="D79" t="s">
+        <v>212</v>
+      </c>
+      <c r="E79" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F79" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>115</v>
       </c>
@@ -4304,14 +5140,21 @@
         <v>309000</v>
       </c>
       <c r="C80">
-        <v>283300</v>
-      </c>
-      <c r="D80" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>327000</v>
+      </c>
+      <c r="D80" t="s">
+        <v>213</v>
+      </c>
+      <c r="E80" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F80" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>116</v>
       </c>
@@ -4319,14 +5162,21 @@
         <v>485500</v>
       </c>
       <c r="C81">
-        <v>443900</v>
-      </c>
-      <c r="D81" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>511000</v>
+      </c>
+      <c r="D81" t="s">
+        <v>214</v>
+      </c>
+      <c r="E81" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F81" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>117</v>
       </c>
@@ -4334,14 +5184,21 @@
         <v>228000</v>
       </c>
       <c r="C82">
-        <v>211000</v>
-      </c>
-      <c r="D82" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>243000</v>
+      </c>
+      <c r="D82" t="s">
+        <v>215</v>
+      </c>
+      <c r="E82" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F82" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>118</v>
       </c>
@@ -4349,14 +5206,21 @@
         <v>157500</v>
       </c>
       <c r="C83">
-        <v>142600</v>
-      </c>
-      <c r="D83" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>170000</v>
+      </c>
+      <c r="D83" t="s">
+        <v>216</v>
+      </c>
+      <c r="E83" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F83" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>119</v>
       </c>
@@ -4364,14 +5228,21 @@
         <v>204000</v>
       </c>
       <c r="C84">
-        <v>193600</v>
-      </c>
-      <c r="D84" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>219000</v>
+      </c>
+      <c r="D84" t="s">
+        <v>159</v>
+      </c>
+      <c r="E84" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F84" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>120</v>
       </c>
@@ -4379,14 +5250,21 @@
         <v>160500</v>
       </c>
       <c r="C85">
-        <v>140000</v>
-      </c>
-      <c r="D85" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172000</v>
+      </c>
+      <c r="D85" t="s">
+        <v>217</v>
+      </c>
+      <c r="E85" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F85" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>121</v>
       </c>
@@ -4394,14 +5272,21 @@
         <v>452000</v>
       </c>
       <c r="C86">
-        <v>402800</v>
-      </c>
-      <c r="D86" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>478500</v>
+      </c>
+      <c r="D86" t="s">
+        <v>218</v>
+      </c>
+      <c r="E86" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F86" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>122</v>
       </c>
@@ -4409,14 +5294,21 @@
         <v>430000</v>
       </c>
       <c r="C87">
-        <v>330200</v>
-      </c>
-      <c r="D87" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>460000</v>
+      </c>
+      <c r="D87" t="s">
+        <v>219</v>
+      </c>
+      <c r="E87" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F87" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>123</v>
       </c>
@@ -4424,14 +5316,21 @@
         <v>366000</v>
       </c>
       <c r="C88">
-        <v>327600</v>
-      </c>
-      <c r="D88" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>386500</v>
+      </c>
+      <c r="D88" t="s">
+        <v>220</v>
+      </c>
+      <c r="E88" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F88" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>124</v>
       </c>
@@ -4439,14 +5338,21 @@
         <v>222000</v>
       </c>
       <c r="C89">
-        <v>199400</v>
-      </c>
-      <c r="D89" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>240000</v>
+      </c>
+      <c r="D89" t="s">
+        <v>221</v>
+      </c>
+      <c r="E89" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F89" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>125</v>
       </c>
@@ -4454,14 +5360,21 @@
         <v>496000</v>
       </c>
       <c r="C90">
-        <v>384000</v>
-      </c>
-      <c r="D90" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>527500</v>
+      </c>
+      <c r="D90" t="s">
+        <v>222</v>
+      </c>
+      <c r="E90" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F90" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>126</v>
       </c>
@@ -4469,14 +5382,21 @@
         <v>339500</v>
       </c>
       <c r="C91">
-        <v>323400</v>
-      </c>
-      <c r="D91" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>360500</v>
+      </c>
+      <c r="D91" t="s">
+        <v>223</v>
+      </c>
+      <c r="E91" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F91" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>127</v>
       </c>
@@ -4484,14 +5404,21 @@
         <v>142000</v>
       </c>
       <c r="C92">
-        <v>92700</v>
-      </c>
-      <c r="D92" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>152000</v>
+      </c>
+      <c r="D92" t="s">
+        <v>224</v>
+      </c>
+      <c r="E92" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F92" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>128</v>
       </c>
@@ -4499,14 +5426,21 @@
         <v>254500</v>
       </c>
       <c r="C93">
-        <v>255200</v>
-      </c>
-      <c r="D93" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>272000</v>
+      </c>
+      <c r="D93" t="s">
+        <v>225</v>
+      </c>
+      <c r="E93" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F93" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>129</v>
       </c>
@@ -4514,14 +5448,21 @@
         <v>323500</v>
       </c>
       <c r="C94">
-        <v>282600</v>
-      </c>
-      <c r="D94" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>345000</v>
+      </c>
+      <c r="D94" t="s">
+        <v>226</v>
+      </c>
+      <c r="E94" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F94" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>130</v>
       </c>
@@ -4529,14 +5470,21 @@
         <v>323000</v>
       </c>
       <c r="C95">
-        <v>276500</v>
-      </c>
-      <c r="D95" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>344000</v>
+      </c>
+      <c r="D95" t="s">
+        <v>227</v>
+      </c>
+      <c r="E95" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F95" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>131</v>
       </c>
@@ -4544,14 +5492,21 @@
         <v>436000</v>
       </c>
       <c r="C96">
-        <v>375700</v>
-      </c>
-      <c r="D96" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>465000</v>
+      </c>
+      <c r="D96" t="s">
+        <v>228</v>
+      </c>
+      <c r="E96" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F96" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>132</v>
       </c>
@@ -4559,14 +5514,21 @@
         <v>359000</v>
       </c>
       <c r="C97">
-        <v>322600</v>
-      </c>
-      <c r="D97" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+        <v>378500</v>
+      </c>
+      <c r="D97" t="s">
+        <v>229</v>
+      </c>
+      <c r="E97" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F97" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>133</v>
       </c>
@@ -4574,14 +5536,21 @@
         <v>186000</v>
       </c>
       <c r="C98">
-        <v>139700</v>
-      </c>
-      <c r="D98" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>197500</v>
+      </c>
+      <c r="D98" t="s">
+        <v>160</v>
+      </c>
+      <c r="E98" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F98" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>134</v>
       </c>
@@ -4589,14 +5558,21 @@
         <v>338000</v>
       </c>
       <c r="C99">
-        <v>323400</v>
-      </c>
-      <c r="D99" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+        <v>362000</v>
+      </c>
+      <c r="D99" t="s">
+        <v>230</v>
+      </c>
+      <c r="E99" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F99" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>135</v>
       </c>
@@ -4604,14 +5580,21 @@
         <v>264000</v>
       </c>
       <c r="C100">
-        <v>245400</v>
-      </c>
-      <c r="D100" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+        <v>282500</v>
+      </c>
+      <c r="D100" t="s">
+        <v>231</v>
+      </c>
+      <c r="E100" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F100" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>136</v>
       </c>
@@ -4619,20 +5602,27 @@
         <v>318000</v>
       </c>
       <c r="C101">
-        <v>285700</v>
-      </c>
-      <c r="D101" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>340000</v>
+      </c>
+      <c r="D101" t="s">
+        <v>232</v>
+      </c>
+      <c r="E101" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F101" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
+  <conditionalFormatting sqref="E102:E1048576 E1:F101">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>